<commit_message>
Main data script with tests and mocks
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/data_test6.xlsx
+++ b/tests/testthat/testdata/data_test6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7F8005-8D84-4AE3-8404-F2942BC84992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB05F5FE-9C09-4CA7-B545-D0E8B49DF8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2685" windowWidth="18900" windowHeight="11160" activeTab="1" xr2:uid="{3F15D76D-AB01-453D-B2EA-47EFBDC62966}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="18900" windowHeight="11160" xr2:uid="{3F15D76D-AB01-453D-B2EA-47EFBDC62966}"/>
   </bookViews>
   <sheets>
     <sheet name="M" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>period</t>
   </si>
@@ -52,6 +52,24 @@
   </si>
   <si>
     <t>UMAR--MZ007--LKJ--11--A</t>
+  </si>
+  <si>
+    <t>1998M01</t>
+  </si>
+  <si>
+    <t>1998M02</t>
+  </si>
+  <si>
+    <t>1998M03</t>
+  </si>
+  <si>
+    <t>1998M04</t>
+  </si>
+  <si>
+    <t>1998M05</t>
+  </si>
+  <si>
+    <t>1998M06</t>
   </si>
 </sst>
 </file>
@@ -406,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55392A8-F2C9-4A16-9210-F27F7AF0B93C}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="A1:D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,8 +445,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1998</v>
+      <c r="A2" t="s">
+        <v>5</v>
       </c>
       <c r="B2">
         <v>32</v>
@@ -441,8 +459,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1999</v>
+      <c r="A3" t="s">
+        <v>6</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -455,8 +473,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2000</v>
+      <c r="A4" t="s">
+        <v>7</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -466,8 +484,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2001</v>
+      <c r="A5" t="s">
+        <v>8</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -477,8 +495,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2002</v>
+      <c r="A6" t="s">
+        <v>9</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -488,8 +506,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2003</v>
+      <c r="A7" t="s">
+        <v>10</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -504,7 +522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1128381-ACD8-4140-9AB1-656C61CEAE3A}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Switch to period input as date and fix downstream.
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/data_test6.xlsx
+++ b/tests/testthat/testdata/data_test6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB05F5FE-9C09-4CA7-B545-D0E8B49DF8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF6C0B1-363E-438F-9530-95A9FE64CFFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="18900" windowHeight="11160" xr2:uid="{3F15D76D-AB01-453D-B2EA-47EFBDC62966}"/>
+    <workbookView xWindow="4380" yWindow="3990" windowWidth="18900" windowHeight="11160" xr2:uid="{3F15D76D-AB01-453D-B2EA-47EFBDC62966}"/>
   </bookViews>
   <sheets>
     <sheet name="M" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>period</t>
   </si>
@@ -52,24 +52,6 @@
   </si>
   <si>
     <t>UMAR--MZ007--LKJ--11--A</t>
-  </si>
-  <si>
-    <t>1998M01</t>
-  </si>
-  <si>
-    <t>1998M02</t>
-  </si>
-  <si>
-    <t>1998M03</t>
-  </si>
-  <si>
-    <t>1998M04</t>
-  </si>
-  <si>
-    <t>1998M05</t>
-  </si>
-  <si>
-    <t>1998M06</t>
   </si>
 </sst>
 </file>
@@ -106,8 +88,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,8 +428,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
+      <c r="A2" s="1">
+        <v>43831</v>
       </c>
       <c r="B2">
         <v>32</v>
@@ -459,8 +442,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
+      <c r="A3" s="1">
+        <v>43862</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -473,8 +456,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
+      <c r="A4" s="1">
+        <v>43891</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -484,8 +467,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
+      <c r="A5" s="1">
+        <v>43922</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -495,8 +478,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
+      <c r="A6" s="1">
+        <v>43952</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -506,8 +489,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
+      <c r="A7" s="1">
+        <v>43983</v>
       </c>
       <c r="B7">
         <v>12</v>

</xml_diff>

<commit_message>
Major refac for new UMARimportr and UMAraccessR functions and type changes on db
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/data_test6.xlsx
+++ b/tests/testthat/testdata/data_test6.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\osebno\ZaloznikM37\bekapiranje\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF6C0B1-363E-438F-9530-95A9FE64CFFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC762DDE-D8BA-4DA4-88E1-48BE276CCC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="3990" windowWidth="18900" windowHeight="11160" xr2:uid="{3F15D76D-AB01-453D-B2EA-47EFBDC62966}"/>
+    <workbookView xWindow="20052" yWindow="-468" windowWidth="23256" windowHeight="12720" xr2:uid="{3F15D76D-AB01-453D-B2EA-47EFBDC62966}"/>
   </bookViews>
   <sheets>
     <sheet name="M" sheetId="1" r:id="rId1"/>
-    <sheet name="A" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,21 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>period</t>
   </si>
   <si>
-    <t>UMAR--MZ001--1123--M</t>
+    <t>UMAR-SURS--MZ002--HR--M</t>
   </si>
   <si>
-    <t>UMAR--MZ001--234--M</t>
-  </si>
-  <si>
-    <t>UMAR--MZ002--1--M</t>
-  </si>
-  <si>
-    <t>UMAR--MZ007--LKJ--11--A</t>
+    <t>UMAR-SURS--MZ002--SI--M</t>
   </si>
 </sst>
 </file>
@@ -109,9 +102,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -149,7 +142,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -255,7 +248,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -397,7 +390,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -405,15 +398,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55392A8-F2C9-4A16-9210-F27F7AF0B93C}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -423,11 +419,8 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43831</v>
       </c>
@@ -437,11 +430,8 @@
       <c r="C2">
         <v>3</v>
       </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43862</v>
       </c>
@@ -451,11 +441,8 @@
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43891</v>
       </c>
@@ -466,7 +453,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43922</v>
       </c>
@@ -477,7 +464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43952</v>
       </c>
@@ -488,80 +475,9 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43983</v>
-      </c>
-      <c r="B7">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1128381-ACD8-4140-9AB1-656C61CEAE3A}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1998</v>
-      </c>
-      <c r="B2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1999</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2000</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2001</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2002</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2003</v>
       </c>
       <c r="B7">
         <v>12</v>

</xml_diff>